<commit_message>
update model performance and comparison
</commit_message>
<xml_diff>
--- a/hepc/data/model_performance.xlsx
+++ b/hepc/data/model_performance.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ONYX\Desktop\data_science\hepc\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE03F3A0-E887-437C-AE23-66A9CACC27F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C01694-41A0-46AA-ACA2-2039906092A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22080" windowHeight="13176" xr2:uid="{24A904DD-1CA2-495C-950A-D125A1FF6801}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22080" windowHeight="13176" activeTab="1" xr2:uid="{24A904DD-1CA2-495C-950A-D125A1FF6801}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="39">
   <si>
     <t>Model</t>
   </si>
@@ -85,6 +86,63 @@
   </si>
   <si>
     <t>SMOTE</t>
+  </si>
+  <si>
+    <t>Cirrhosis</t>
+  </si>
+  <si>
+    <t>Fibrosis</t>
+  </si>
+  <si>
+    <t>Hepatitis</t>
+  </si>
+  <si>
+    <t>Blood Donor</t>
+  </si>
+  <si>
+    <t>Validation Sample</t>
+  </si>
+  <si>
+    <t>Classifier Index</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>selected</t>
+  </si>
+  <si>
+    <t>2.3.cost.1000</t>
+  </si>
+  <si>
+    <t>2.1.cost.1000</t>
+  </si>
+  <si>
+    <t>3.1.no_weights</t>
+  </si>
+  <si>
+    <t>4.1.no_weights</t>
+  </si>
+  <si>
+    <t>Model 2</t>
+  </si>
+  <si>
+    <t>Model 3</t>
+  </si>
+  <si>
+    <t>Model 4</t>
+  </si>
+  <si>
+    <t>Correctly Classified (Count)</t>
+  </si>
+  <si>
+    <t>Wrongly Classified (Count)</t>
+  </si>
+  <si>
+    <t>Percentage Correctly Classified</t>
+  </si>
+  <si>
+    <t>Stages</t>
   </si>
 </sst>
 </file>
@@ -94,7 +152,14 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,7 +168,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -116,8 +181,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -225,11 +314,61 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -261,11 +400,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="62">
+  <dxfs count="31">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -308,41 +488,11 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="4"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -357,376 +507,13 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0000"/>
@@ -903,6 +690,22 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -923,6 +726,23 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -943,6 +763,22 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -963,6 +799,7 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -973,7 +810,39 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1062,22 +931,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A1BF736A-829E-4848-BC08-3A80826D7F43}" name="Table1" displayName="Table1" ref="A1:J22" headerRowDxfId="61" headerRowBorderDxfId="60" tableBorderDxfId="59" totalsRowBorderDxfId="58">
-  <autoFilter ref="A1:J22" xr:uid="{7A905A65-2751-434E-8861-D2134C65A31F}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A1BF736A-829E-4848-BC08-3A80826D7F43}" name="Table1" displayName="Table1" ref="A1:K22" headerRowDxfId="30" headerRowBorderDxfId="29" tableBorderDxfId="28" totalsRowBorderDxfId="27">
+  <autoFilter ref="A1:K22" xr:uid="{9F9B803E-7B08-45EB-A48B-84C3602A4472}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K22">
     <sortCondition descending="1" ref="H1:H22"/>
   </sortState>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{03097363-BA46-44C6-A5E4-18E291AE1E8C}" name="No" dataDxfId="57" totalsRowDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{FA79F0C7-E4A5-4955-994D-F7B662727205}" name="Model" dataDxfId="42" totalsRowDxfId="55"/>
-    <tableColumn id="10" xr3:uid="{1914F1C3-48A5-4C64-8680-8E407730F0A2}" name="Oversampling" dataDxfId="41" totalsRowDxfId="54"/>
-    <tableColumn id="3" xr3:uid="{928D0B71-EDCB-4A51-8D31-3A8ED6189731}" name="Feature Used" dataDxfId="40" totalsRowDxfId="53"/>
-    <tableColumn id="4" xr3:uid="{E961CC29-4C77-4A5D-B21F-4DF73DC281B8}" name="Class Weight" dataDxfId="38" totalsRowDxfId="52"/>
-    <tableColumn id="5" xr3:uid="{8B9641AF-CBF2-4E41-BD22-E31494BC02E8}" name="Kernel" dataDxfId="39" totalsRowDxfId="51"/>
-    <tableColumn id="6" xr3:uid="{73B6A57D-B173-4D65-AA8D-2B5989298892}" name="C" dataDxfId="50" totalsRowDxfId="49"/>
-    <tableColumn id="7" xr3:uid="{9F82A6A2-AC64-4CE6-8055-6359DC02BD95}" name="Balanced Accuracy" dataDxfId="48" totalsRowDxfId="47"/>
-    <tableColumn id="8" xr3:uid="{EBD65853-F67D-457C-ACD3-1634791C6640}" name="Sensitivity" dataDxfId="46" totalsRowDxfId="45"/>
-    <tableColumn id="9" xr3:uid="{31DB3BB9-FE24-40C1-B83F-18FDE1453E82}" name="Specificity" dataDxfId="44" totalsRowDxfId="43"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{03097363-BA46-44C6-A5E4-18E291AE1E8C}" name="No" dataDxfId="26" totalsRowDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{FA79F0C7-E4A5-4955-994D-F7B662727205}" name="Model" dataDxfId="24" totalsRowDxfId="23"/>
+    <tableColumn id="10" xr3:uid="{1914F1C3-48A5-4C64-8680-8E407730F0A2}" name="Oversampling" dataDxfId="22" totalsRowDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{928D0B71-EDCB-4A51-8D31-3A8ED6189731}" name="Feature Used" dataDxfId="20" totalsRowDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{E961CC29-4C77-4A5D-B21F-4DF73DC281B8}" name="Class Weight" dataDxfId="18" totalsRowDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{8B9641AF-CBF2-4E41-BD22-E31494BC02E8}" name="Kernel" dataDxfId="16" totalsRowDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{73B6A57D-B173-4D65-AA8D-2B5989298892}" name="C" dataDxfId="14" totalsRowDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{9F82A6A2-AC64-4CE6-8055-6359DC02BD95}" name="Balanced Accuracy" dataDxfId="12" totalsRowDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{EBD65853-F67D-457C-ACD3-1634791C6640}" name="Sensitivity" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{31DB3BB9-FE24-40C1-B83F-18FDE1453E82}" name="Specificity" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{D4F0E71C-2118-4933-8D89-30A286CC37A3}" name="Classifier Index" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1380,10 +1250,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50BB58C3-1433-4CC0-B8F5-BAC69067429C}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1398,10 +1268,11 @@
     <col min="8" max="8" width="19.109375" style="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.77734375" style="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.77734375" style="11" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="11"/>
+    <col min="11" max="11" width="15.77734375" style="25" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>16</v>
       </c>
@@ -1432,8 +1303,11 @@
       <c r="J1" s="7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K1" s="24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1464,8 +1338,11 @@
       <c r="J2" s="4">
         <v>0.93079999999999996</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K2" s="25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1496,8 +1373,11 @@
       <c r="J3" s="4">
         <v>0.92449999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K3" s="25">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="18">
         <v>3</v>
       </c>
@@ -1528,8 +1408,11 @@
       <c r="J4" s="14">
         <v>0.98109999999999997</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K4" s="25">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="18">
         <v>4</v>
       </c>
@@ -1560,8 +1443,11 @@
       <c r="J5" s="14">
         <v>0.94969999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K5" s="25">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1592,8 +1478,11 @@
       <c r="J6" s="4">
         <v>0.98741999999999996</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K6" s="25">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1624,8 +1513,11 @@
       <c r="J7" s="14">
         <v>0.94969000000000003</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K7" s="25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1656,8 +1548,11 @@
       <c r="J8" s="4">
         <v>0.98109999999999997</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K8" s="25">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="18">
         <v>8</v>
       </c>
@@ -1688,8 +1583,11 @@
       <c r="J9" s="4">
         <v>0.98109999999999997</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K9" s="25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="18">
         <v>9</v>
       </c>
@@ -1720,8 +1618,11 @@
       <c r="J10" s="17">
         <v>0.96860000000000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K10" s="25">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1752,8 +1653,11 @@
       <c r="J11" s="14">
         <v>0.93710000000000004</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K11" s="25">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1784,8 +1688,11 @@
       <c r="J12" s="14">
         <v>0.96855000000000002</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K12" s="25">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1816,8 +1723,11 @@
       <c r="J13" s="4">
         <v>0.99370999999999998</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K13" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="18">
         <v>13</v>
       </c>
@@ -1848,8 +1758,11 @@
       <c r="J14" s="14">
         <v>0.98112999999999995</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K14" s="25">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="18">
         <v>14</v>
       </c>
@@ -1880,8 +1793,11 @@
       <c r="J15" s="17">
         <v>0.96855000000000002</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K15" s="25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1912,8 +1828,11 @@
       <c r="J16" s="10">
         <v>0.98741999999999996</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K16" s="25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1944,8 +1863,11 @@
       <c r="J17" s="17">
         <v>0.92452999999999996</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K17" s="25">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -1976,8 +1898,11 @@
       <c r="J18" s="17">
         <v>0.96855000000000002</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K18" s="25">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="18">
         <v>18</v>
       </c>
@@ -2008,8 +1933,11 @@
       <c r="J19" s="4">
         <v>0.91195000000000004</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K19" s="25">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="18">
         <v>19</v>
       </c>
@@ -2040,8 +1968,11 @@
       <c r="J20" s="14">
         <v>0.99370999999999998</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K20" s="25">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2072,8 +2003,11 @@
       <c r="J21" s="4">
         <v>0.81132000000000004</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K21" s="25">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -2103,6 +2037,9 @@
       </c>
       <c r="J22" s="14">
         <v>0.98112999999999995</v>
+      </c>
+      <c r="K22" s="25">
+        <v>4.3</v>
       </c>
     </row>
   </sheetData>
@@ -2149,25 +2086,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C22">
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+      <formula>"ROSE"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
       <formula>"SMOTE"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
-      <formula>"ROSE"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F22">
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
-      <formula>"Linear"</formula>
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"Sigmoid"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Polynomial">
+      <formula>NOT(ISERROR(SEARCH("Polynomial",F2)))</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"Radial"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Polynomial">
-      <formula>NOT(ISERROR(SEARCH("Polynomial",F2)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
-      <formula>"Sigmoid"</formula>
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+      <formula>"Linear"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2221,4 +2158,261 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{228C3036-6AE1-4C97-97A3-1A2074BAD4EF}">
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="10.44140625" style="11" customWidth="1"/>
+    <col min="6" max="11" width="10" style="11" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="28"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="45" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="52">
+        <v>11</v>
+      </c>
+      <c r="C3" s="29">
+        <v>11</v>
+      </c>
+      <c r="D3" s="15">
+        <v>9</v>
+      </c>
+      <c r="E3" s="39">
+        <v>11</v>
+      </c>
+      <c r="F3" s="15">
+        <f>$B3-C3</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="39">
+        <f>$B3-D3</f>
+        <v>2</v>
+      </c>
+      <c r="H3" s="15">
+        <f>$B3-E3</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="40">
+        <f>C3/$B3</f>
+        <v>1</v>
+      </c>
+      <c r="J3" s="49">
+        <f>D3/$B3</f>
+        <v>0.81818181818181823</v>
+      </c>
+      <c r="K3" s="41">
+        <f>E3/$B3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="32">
+        <v>3</v>
+      </c>
+      <c r="C4" s="29">
+        <v>3</v>
+      </c>
+      <c r="D4" s="31">
+        <v>3</v>
+      </c>
+      <c r="E4" s="29">
+        <v>3</v>
+      </c>
+      <c r="F4" s="31">
+        <f>$B4-C4</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="29">
+        <f>$B4-D4</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="31">
+        <f>$B4-E4</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="38">
+        <f>C4/$B4</f>
+        <v>1</v>
+      </c>
+      <c r="J4" s="50">
+        <f>D4/$B4</f>
+        <v>1</v>
+      </c>
+      <c r="K4" s="42">
+        <f>E4/$B4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="32">
+        <v>8</v>
+      </c>
+      <c r="C5" s="29">
+        <v>6</v>
+      </c>
+      <c r="D5" s="31">
+        <v>7</v>
+      </c>
+      <c r="E5" s="29">
+        <v>5</v>
+      </c>
+      <c r="F5" s="31">
+        <f>$B5-C5</f>
+        <v>2</v>
+      </c>
+      <c r="G5" s="29">
+        <f>$B5-D5</f>
+        <v>1</v>
+      </c>
+      <c r="H5" s="31">
+        <f>$B5-E5</f>
+        <v>3</v>
+      </c>
+      <c r="I5" s="38">
+        <f>C5/$B5</f>
+        <v>0.75</v>
+      </c>
+      <c r="J5" s="50">
+        <f>D5/$B5</f>
+        <v>0.875</v>
+      </c>
+      <c r="K5" s="42">
+        <f>E5/$B5</f>
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="33">
+        <v>159</v>
+      </c>
+      <c r="C6" s="35">
+        <v>147</v>
+      </c>
+      <c r="D6" s="23">
+        <v>156</v>
+      </c>
+      <c r="E6" s="35">
+        <v>151</v>
+      </c>
+      <c r="F6" s="23">
+        <f>$B6-C6</f>
+        <v>12</v>
+      </c>
+      <c r="G6" s="35">
+        <f>$B6-D6</f>
+        <v>3</v>
+      </c>
+      <c r="H6" s="23">
+        <f>$B6-E6</f>
+        <v>8</v>
+      </c>
+      <c r="I6" s="43">
+        <f>C6/$B6</f>
+        <v>0.92452830188679247</v>
+      </c>
+      <c r="J6" s="51">
+        <f>D6/$B6</f>
+        <v>0.98113207547169812</v>
+      </c>
+      <c r="K6" s="44">
+        <f>E6/$B6</f>
+        <v>0.94968553459119498</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="A1:A2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="I3:K6">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>